<commit_message>
fixed attribute entity mappings and added Location entity
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="-160" yWindow="0" windowWidth="25360" windowHeight="14540" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
-    <sheet name="TypeTestRef" sheetId="2" r:id="rId2"/>
+    <sheet name="test_TypeTest" sheetId="1" r:id="rId1"/>
+    <sheet name="test_TypeTestRef" sheetId="2" r:id="rId2"/>
     <sheet name="packages" sheetId="5" r:id="rId3"/>
     <sheet name="entities" sheetId="3" r:id="rId4"/>
     <sheet name="attributes" sheetId="4" r:id="rId5"/>
+    <sheet name="test_Location" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="162">
   <si>
     <t>text</t>
   </si>
@@ -448,12 +449,6 @@
     <t>package</t>
   </si>
   <si>
-    <t>molgenis</t>
-  </si>
-  <si>
-    <t>org</t>
-  </si>
-  <si>
     <t>xcomputedint</t>
   </si>
   <si>
@@ -503,6 +498,18 @@
   </si>
   <si>
     <t>xcategoricalmrefnillable</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>test_TypeTestRef</t>
+  </si>
+  <si>
+    <t>test_TypeTest</t>
+  </si>
+  <si>
+    <t>test_Location</t>
   </si>
 </sst>
 </file>
@@ -558,9 +565,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -577,7 +587,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -587,6 +597,9 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -889,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AH28" sqref="AH28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -898,7 +911,7 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
@@ -933,10 +946,10 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
@@ -945,10 +958,10 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -1070,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -1204,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -1335,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1418,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -1552,7 +1565,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -1683,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -1763,7 +1776,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -1894,7 +1907,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -2022,7 +2035,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -2102,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -2233,7 +2246,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -2361,7 +2374,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
@@ -2441,7 +2454,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
         <v>2</v>
@@ -2572,7 +2585,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
@@ -2700,7 +2713,7 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
@@ -2777,7 +2790,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
@@ -2857,7 +2870,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -2988,7 +3001,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -3116,7 +3129,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -3196,7 +3209,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
@@ -3327,7 +3340,7 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -3452,7 +3465,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -3529,7 +3542,7 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -3657,7 +3670,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F25" t="s">
         <v>3</v>
@@ -3782,7 +3795,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -3859,7 +3872,7 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F27" t="s">
         <v>2</v>
@@ -3987,7 +4000,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
         <v>3</v>
@@ -4112,7 +4125,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -4189,7 +4202,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F30" t="s">
         <v>2</v>
@@ -4317,7 +4330,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -4442,7 +4455,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -4519,7 +4532,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F33" t="s">
         <v>2</v>
@@ -4647,7 +4660,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F34" t="s">
         <v>3</v>
@@ -4772,7 +4785,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
@@ -4846,7 +4859,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
@@ -4923,7 +4936,7 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F37" t="s">
         <v>2</v>
@@ -5051,7 +5064,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F38" t="s">
         <v>3</v>
@@ -5176,7 +5189,7 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F39" t="s">
         <v>4</v>
@@ -5380,7 +5393,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD50"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5445,10 +5458,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A100"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5456,7 +5469,7 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5466,33 +5479,21 @@
       <c r="C1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>138</v>
       </c>
       <c r="B2" t="s">
         <v>139</v>
       </c>
-      <c r="C2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>142</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5506,7 +5507,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5527,7 +5528,7 @@
         <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5551,7 +5552,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -5568,8 +5572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5579,8 +5583,11 @@
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" customWidth="1"/>
     <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5631,10 +5638,10 @@
         <v>99</v>
       </c>
       <c r="P1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -5642,7 +5649,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>66</v>
@@ -5662,7 +5669,7 @@
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
@@ -5685,7 +5692,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C4" t="s">
         <v>67</v>
@@ -5705,7 +5712,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -5725,7 +5732,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -5742,13 +5749,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -5759,10 +5766,10 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
@@ -5777,15 +5784,15 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C9" t="s">
         <v>66</v>
@@ -5800,7 +5807,7 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -5808,13 +5815,13 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -5828,13 +5835,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -5845,16 +5852,16 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -5868,16 +5875,16 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" t="s">
         <v>159</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -5891,7 +5898,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C14" t="s">
         <v>70</v>
@@ -5911,7 +5918,7 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
         <v>70</v>
@@ -5928,7 +5935,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
         <v>71</v>
@@ -5945,7 +5952,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
@@ -5965,7 +5972,7 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
@@ -5985,7 +5992,7 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -6002,7 +6009,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
         <v>73</v>
@@ -6022,7 +6029,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
         <v>73</v>
@@ -6039,7 +6046,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C22" t="s">
         <v>80</v>
@@ -6062,7 +6069,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
@@ -6082,7 +6089,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
@@ -6099,7 +6106,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
@@ -6119,7 +6126,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C26" t="s">
         <v>75</v>
@@ -6139,7 +6146,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
         <v>75</v>
@@ -6156,7 +6163,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
@@ -6176,7 +6183,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
@@ -6193,7 +6200,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
         <v>67</v>
@@ -6216,7 +6223,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
         <v>67</v>
@@ -6239,7 +6246,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -6256,7 +6263,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -6273,7 +6280,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -6299,7 +6306,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -6325,13 +6332,13 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C36" t="s">
         <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -6348,13 +6355,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C37" t="s">
         <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -6368,7 +6375,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -6388,7 +6395,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -6405,7 +6412,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -6422,7 +6429,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -6439,13 +6446,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s">
         <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -6462,13 +6469,13 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C43" t="s">
         <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -6482,7 +6489,7 @@
         <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
         <v>66</v>
@@ -6502,7 +6509,7 @@
         <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C45" t="s">
         <v>66</v>
@@ -6522,7 +6529,7 @@
         <v>98</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C46" t="s">
         <v>66</v>
@@ -6542,7 +6549,7 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C47" t="s">
         <v>67</v>
@@ -6562,13 +6569,13 @@
         <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
         <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -6582,16 +6589,16 @@
     </row>
     <row r="49" spans="1:17">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -6603,15 +6610,15 @@
         <v>1</v>
       </c>
       <c r="Q49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
       <c r="C50" t="s">
         <v>67</v>
@@ -6631,10 +6638,10 @@
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>66</v>
@@ -6660,10 +6667,10 @@
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>67</v>
@@ -6696,4 +6703,56 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>